<commit_message>
Completed basic parser of simple equations featuring mul, div, add, sub, mod
</commit_message>
<xml_diff>
--- a/src/main/resources/documents/ToDo.xlsx
+++ b/src/main/resources/documents/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Website\website-backend\src\main\resources\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0092E78-E489-4ED6-8FC2-388D883E8856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008588F8-4BC4-4CF9-910F-BC666E822A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17250" yWindow="1260" windowWidth="6615" windowHeight="13500" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -474,10 +474,14 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Added big-decimal support. (#21)
</commit_message>
<xml_diff>
--- a/src/main/resources/documents/ToDo.xlsx
+++ b/src/main/resources/documents/ToDo.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Website\website-backend\src\main\resources\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008588F8-4BC4-4CF9-910F-BC666E822A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0227A375-4F87-4830-9286-8F1D64E253EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
+    <workbookView xWindow="2730" yWindow="2700" windowWidth="21600" windowHeight="11505" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
+    <sheet name="Constants" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="89">
   <si>
     <t>Number</t>
   </si>
@@ -120,6 +121,186 @@
   </si>
   <si>
     <t>sqrt(a)</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Log N</t>
+  </si>
+  <si>
+    <t>log 2</t>
+  </si>
+  <si>
+    <t>log e</t>
+  </si>
+  <si>
+    <t>log 10</t>
+  </si>
+  <si>
+    <t>rng(a, b)</t>
+  </si>
+  <si>
+    <t>FLOOR</t>
+  </si>
+  <si>
+    <t>CEIL</t>
+  </si>
+  <si>
+    <t>LN</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>LOG</t>
+  </si>
+  <si>
+    <t>LOGN</t>
+  </si>
+  <si>
+    <t>RNG</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>max(a1, a2, …, aN)</t>
+  </si>
+  <si>
+    <t>CHOOSE</t>
+  </si>
+  <si>
+    <t>PERM</t>
+  </si>
+  <si>
+    <t>Random integer a &lt;= n &lt; b</t>
+  </si>
+  <si>
+    <t>Random float a &lt;= n &lt; b</t>
+  </si>
+  <si>
+    <t>TANGENT</t>
+  </si>
+  <si>
+    <t>tan(a)</t>
+  </si>
+  <si>
+    <t>rngf(a, b)</t>
+  </si>
+  <si>
+    <t>RNG_FLOAT</t>
+  </si>
+  <si>
+    <t>atan(a)</t>
+  </si>
+  <si>
+    <t>asin(a)</t>
+  </si>
+  <si>
+    <t>acos(a)</t>
+  </si>
+  <si>
+    <t>htan(a)</t>
+  </si>
+  <si>
+    <t>hsin(a)</t>
+  </si>
+  <si>
+    <t>hcos(a)</t>
+  </si>
+  <si>
+    <t>TANGENT_INVERSE</t>
+  </si>
+  <si>
+    <t>SINE_INVERSE</t>
+  </si>
+  <si>
+    <t>COSINE_INVERSE</t>
+  </si>
+  <si>
+    <t>TANGENT_HYPERBOLIC</t>
+  </si>
+  <si>
+    <t>SINE_HYPERBOLIC</t>
+  </si>
+  <si>
+    <t>COSINE_HYPERBOLIC</t>
+  </si>
+  <si>
+    <t>COSECANT</t>
+  </si>
+  <si>
+    <t>SECANT</t>
+  </si>
+  <si>
+    <t>COTANGENT</t>
+  </si>
+  <si>
+    <t>SECANT_INVERSE</t>
+  </si>
+  <si>
+    <t>COSECANT_INVERSE</t>
+  </si>
+  <si>
+    <t>COTANGENT_INVERSE</t>
+  </si>
+  <si>
+    <t>SECANT_HYPERBOLIC</t>
+  </si>
+  <si>
+    <t>COSECANT_HYPERBOLIC</t>
+  </si>
+  <si>
+    <t>COTANGENT_HYPERBOLIC</t>
+  </si>
+  <si>
+    <t>GCD</t>
+  </si>
+  <si>
+    <t>LCM</t>
+  </si>
+  <si>
+    <t>Greatest common divisor</t>
+  </si>
+  <si>
+    <t>Least common multiple</t>
+  </si>
+  <si>
+    <t>sec(a)</t>
+  </si>
+  <si>
+    <t>cot(a)</t>
+  </si>
+  <si>
+    <t>csc(a)</t>
+  </si>
+  <si>
+    <t>asec(a)</t>
+  </si>
+  <si>
+    <t>acsc(a)</t>
+  </si>
+  <si>
+    <t>acot(a)</t>
+  </si>
+  <si>
+    <t>hsec(a)</t>
+  </si>
+  <si>
+    <t>hcot(a)</t>
+  </si>
+  <si>
+    <t>gcd(a1, a2, …, aN)</t>
+  </si>
+  <si>
+    <t>lcm(a1, a2, …, aN)</t>
   </si>
 </sst>
 </file>
@@ -161,7 +342,38 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -471,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BCC905-A409-42C2-89DD-4C1C7079AB36}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,6 +722,9 @@
       <c r="C2" t="s">
         <v>15</v>
       </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -521,6 +736,9 @@
       <c r="C3" t="s">
         <v>16</v>
       </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -532,6 +750,9 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -543,6 +764,9 @@
       <c r="C5" t="s">
         <v>18</v>
       </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -554,6 +778,9 @@
       <c r="C6" t="s">
         <v>20</v>
       </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -565,6 +792,9 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -576,6 +806,9 @@
       <c r="C8" t="s">
         <v>22</v>
       </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -587,6 +820,9 @@
       <c r="C9" t="s">
         <v>23</v>
       </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -598,6 +834,9 @@
       <c r="C10" t="s">
         <v>24</v>
       </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -609,6 +848,9 @@
       <c r="C11" t="s">
         <v>25</v>
       </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -620,6 +862,9 @@
       <c r="C12" t="s">
         <v>26</v>
       </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -631,94 +876,452 @@
       <c r="C13" t="s">
         <v>28</v>
       </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" t="s">
+        <v>30</v>
+      </c>
+      <c r="F42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" t="s">
+        <v>30</v>
+      </c>
+      <c r="F43" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="N?A">
+      <formula>NOT(ISERROR(SEARCH("N?A",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="IP">
+      <formula>NOT(ISERROR(SEARCH("IP",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43B3F45-0AB1-4877-8E90-17E1166AA05D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Started to add parsing. Need to work with n-type functions.
</commit_message>
<xml_diff>
--- a/src/main/resources/documents/ToDo.xlsx
+++ b/src/main/resources/documents/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Website\website-backend\src\main\resources\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0227A375-4F87-4830-9286-8F1D64E253EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2F1876-EA8E-4ABB-A0D4-2860853FAA9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2700" windowWidth="21600" windowHeight="11505" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
+    <workbookView xWindow="12780" yWindow="1470" windowWidth="21600" windowHeight="11505" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="90">
   <si>
     <t>Number</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>lcm(a1, a2, …, aN)</t>
+  </si>
+  <si>
+    <t>IP</t>
   </si>
 </sst>
 </file>
@@ -686,12 +689,12 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -807,7 +810,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -957,7 +960,7 @@
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="F20" t="s">
         <v>33</v>
@@ -971,7 +974,7 @@
         <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="F21" t="s">
         <v>32</v>
@@ -985,7 +988,7 @@
         <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="F22" t="s">
         <v>34</v>
@@ -999,7 +1002,7 @@
         <v>41</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="F23" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Add Function Parsing from JSON (#26)
* Added ability to parse n-param functions from JSON
</commit_message>
<xml_diff>
--- a/src/main/resources/documents/ToDo.xlsx
+++ b/src/main/resources/documents/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Website\website-backend\src\main\resources\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0227A375-4F87-4830-9286-8F1D64E253EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2F1876-EA8E-4ABB-A0D4-2860853FAA9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2700" windowWidth="21600" windowHeight="11505" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
+    <workbookView xWindow="12780" yWindow="1470" windowWidth="21600" windowHeight="11505" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="90">
   <si>
     <t>Number</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>lcm(a1, a2, …, aN)</t>
+  </si>
+  <si>
+    <t>IP</t>
   </si>
 </sst>
 </file>
@@ -686,12 +689,12 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -807,7 +810,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -957,7 +960,7 @@
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="F20" t="s">
         <v>33</v>
@@ -971,7 +974,7 @@
         <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="F21" t="s">
         <v>32</v>
@@ -985,7 +988,7 @@
         <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="F22" t="s">
         <v>34</v>
@@ -999,7 +1002,7 @@
         <v>41</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="F23" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Cleaned up the code, added power and modPow
</commit_message>
<xml_diff>
--- a/src/main/resources/documents/ToDo.xlsx
+++ b/src/main/resources/documents/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Website\website-backend\src\main\resources\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2F1876-EA8E-4ABB-A0D4-2860853FAA9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955F1A54-8C9A-4250-A937-26B7FA63EA07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="1470" windowWidth="21600" windowHeight="11505" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
+    <workbookView xWindow="41100" yWindow="90" windowWidth="28800" windowHeight="15555" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="95">
   <si>
     <t>Number</t>
   </si>
@@ -304,6 +304,21 @@
   </si>
   <si>
     <t>IP</t>
+  </si>
+  <si>
+    <t>min(a1, a2, …, aN)</t>
+  </si>
+  <si>
+    <t>ROUND</t>
+  </si>
+  <si>
+    <t>round(a, accuracy)</t>
+  </si>
+  <si>
+    <t>MOD_POWER</t>
+  </si>
+  <si>
+    <t>modPow(base, exp, mod)</t>
   </si>
 </sst>
 </file>
@@ -686,15 +701,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BCC905-A409-42C2-89DD-4C1C7079AB36}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -810,7 +826,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -904,8 +920,11 @@
       <c r="B15" t="s">
         <v>44</v>
       </c>
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -938,7 +957,7 @@
         <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -949,7 +968,7 @@
         <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -960,7 +979,7 @@
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="F20" t="s">
         <v>33</v>
@@ -974,7 +993,7 @@
         <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="F21" t="s">
         <v>32</v>
@@ -988,7 +1007,7 @@
         <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="F22" t="s">
         <v>34</v>
@@ -1002,7 +1021,7 @@
         <v>41</v>
       </c>
       <c r="D23" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="F23" t="s">
         <v>31</v>
@@ -1019,7 +1038,7 @@
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F24" t="s">
         <v>48</v>
@@ -1036,7 +1055,7 @@
         <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="F25" t="s">
         <v>49</v>
@@ -1298,6 +1317,34 @@
       </c>
       <c r="F43" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Functions and Error Checking (#27)
* Add randint function.

* Cleaned up the code, added power and modPow
</commit_message>
<xml_diff>
--- a/src/main/resources/documents/ToDo.xlsx
+++ b/src/main/resources/documents/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Website\website-backend\src\main\resources\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2F1876-EA8E-4ABB-A0D4-2860853FAA9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955F1A54-8C9A-4250-A937-26B7FA63EA07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="1470" windowWidth="21600" windowHeight="11505" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
+    <workbookView xWindow="41100" yWindow="90" windowWidth="28800" windowHeight="15555" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="95">
   <si>
     <t>Number</t>
   </si>
@@ -304,6 +304,21 @@
   </si>
   <si>
     <t>IP</t>
+  </si>
+  <si>
+    <t>min(a1, a2, …, aN)</t>
+  </si>
+  <si>
+    <t>ROUND</t>
+  </si>
+  <si>
+    <t>round(a, accuracy)</t>
+  </si>
+  <si>
+    <t>MOD_POWER</t>
+  </si>
+  <si>
+    <t>modPow(base, exp, mod)</t>
   </si>
 </sst>
 </file>
@@ -686,15 +701,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BCC905-A409-42C2-89DD-4C1C7079AB36}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -810,7 +826,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -904,8 +920,11 @@
       <c r="B15" t="s">
         <v>44</v>
       </c>
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -938,7 +957,7 @@
         <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -949,7 +968,7 @@
         <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -960,7 +979,7 @@
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="F20" t="s">
         <v>33</v>
@@ -974,7 +993,7 @@
         <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="F21" t="s">
         <v>32</v>
@@ -988,7 +1007,7 @@
         <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="F22" t="s">
         <v>34</v>
@@ -1002,7 +1021,7 @@
         <v>41</v>
       </c>
       <c r="D23" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="F23" t="s">
         <v>31</v>
@@ -1019,7 +1038,7 @@
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F24" t="s">
         <v>48</v>
@@ -1036,7 +1055,7 @@
         <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="F25" t="s">
         <v>49</v>
@@ -1298,6 +1317,34 @@
       </c>
       <c r="F43" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added integer division and factorial -- easier than I had thought :)
</commit_message>
<xml_diff>
--- a/src/main/resources/documents/ToDo.xlsx
+++ b/src/main/resources/documents/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Website\website-backend\src\main\resources\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955F1A54-8C9A-4250-A937-26B7FA63EA07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E26BA43-287E-4BAC-B4D1-50930F6684AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41100" yWindow="90" windowWidth="28800" windowHeight="15555" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
+    <workbookView xWindow="4395" yWindow="4155" windowWidth="21600" windowHeight="11505" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BCC905-A409-42C2-89DD-4C1C7079AB36}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E45" sqref="A45:XFD45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +798,7 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -826,7 +826,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -840,7 +840,7 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -868,7 +868,7 @@
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -882,7 +882,7 @@
         <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1072,7 +1072,7 @@
         <v>51</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
         <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1100,7 +1100,7 @@
         <v>55</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1114,7 +1114,7 @@
         <v>56</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1128,7 +1128,7 @@
         <v>57</v>
       </c>
       <c r="D30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1142,7 +1142,7 @@
         <v>58</v>
       </c>
       <c r="D31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
         <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1170,7 +1170,7 @@
         <v>79</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1184,7 +1184,7 @@
         <v>81</v>
       </c>
       <c r="D34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1198,7 +1198,7 @@
         <v>80</v>
       </c>
       <c r="D35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1212,7 +1212,7 @@
         <v>82</v>
       </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1226,7 +1226,7 @@
         <v>83</v>
       </c>
       <c r="D37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1240,7 +1240,7 @@
         <v>84</v>
       </c>
       <c r="D38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1254,7 +1254,7 @@
         <v>85</v>
       </c>
       <c r="D39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1268,7 +1268,7 @@
         <v>59</v>
       </c>
       <c r="D40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1282,7 +1282,7 @@
         <v>86</v>
       </c>
       <c r="D41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1296,7 +1296,7 @@
         <v>87</v>
       </c>
       <c r="D42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F42" t="s">
         <v>77</v>
@@ -1313,7 +1313,7 @@
         <v>88</v>
       </c>
       <c r="D43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F43" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
Add GCD, LCM, Integer Division, and Factorial (#30)
* Implemented basic GCD

* Added integer division and factorial -- easier than I had thought :)
</commit_message>
<xml_diff>
--- a/src/main/resources/documents/ToDo.xlsx
+++ b/src/main/resources/documents/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Website\website-backend\src\main\resources\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955F1A54-8C9A-4250-A937-26B7FA63EA07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E26BA43-287E-4BAC-B4D1-50930F6684AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41100" yWindow="90" windowWidth="28800" windowHeight="15555" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
+    <workbookView xWindow="4395" yWindow="4155" windowWidth="21600" windowHeight="11505" xr2:uid="{81D0F296-904F-4176-88A9-C6A03BB3E33D}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BCC905-A409-42C2-89DD-4C1C7079AB36}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E45" sqref="A45:XFD45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +798,7 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -826,7 +826,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -840,7 +840,7 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -868,7 +868,7 @@
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -882,7 +882,7 @@
         <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1072,7 +1072,7 @@
         <v>51</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
         <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1100,7 +1100,7 @@
         <v>55</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1114,7 +1114,7 @@
         <v>56</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1128,7 +1128,7 @@
         <v>57</v>
       </c>
       <c r="D30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1142,7 +1142,7 @@
         <v>58</v>
       </c>
       <c r="D31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
         <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1170,7 +1170,7 @@
         <v>79</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1184,7 +1184,7 @@
         <v>81</v>
       </c>
       <c r="D34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1198,7 +1198,7 @@
         <v>80</v>
       </c>
       <c r="D35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1212,7 +1212,7 @@
         <v>82</v>
       </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1226,7 +1226,7 @@
         <v>83</v>
       </c>
       <c r="D37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1240,7 +1240,7 @@
         <v>84</v>
       </c>
       <c r="D38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1254,7 +1254,7 @@
         <v>85</v>
       </c>
       <c r="D39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1268,7 +1268,7 @@
         <v>59</v>
       </c>
       <c r="D40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1282,7 +1282,7 @@
         <v>86</v>
       </c>
       <c r="D41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1296,7 +1296,7 @@
         <v>87</v>
       </c>
       <c r="D42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F42" t="s">
         <v>77</v>
@@ -1313,7 +1313,7 @@
         <v>88</v>
       </c>
       <c r="D43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F43" t="s">
         <v>78</v>

</xml_diff>